<commit_message>
Updated report to user
</commit_message>
<xml_diff>
--- a/GameGetter/Data/Input/EpicGameList.xlsx
+++ b/GameGetter/Data/Input/EpicGameList.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
   <x:si>
     <x:t>Title</x:t>
   </x:si>
@@ -49,13 +49,88 @@
     <x:t>Title_2_1</x:t>
   </x:si>
   <x:si>
+    <x:t>URL_1_1</x:t>
+  </x:si>
+  <x:si>
     <x:t>Status_2_1</x:t>
   </x:si>
   <x:si>
-    <x:t>The Cycle</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://www.epicgames.com/store/en-US/product/thecycle/home</x:t>
+    <x:t>Title_1_1_1</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Status_1_1_1</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Title_2_1_1</x:t>
+  </x:si>
+  <x:si>
+    <x:t>URL_1_1_1</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Status_2_1_1</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Title_1_1_1_1</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Status_1_1_1_1</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Title_2_1_1_1</x:t>
+  </x:si>
+  <x:si>
+    <x:t>URL_1_1_1_1</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Status_2_1_1_1</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Title_1_1_1_1_1</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Status_1_1_1_1_1</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Title_2_1_1_1_1</x:t>
+  </x:si>
+  <x:si>
+    <x:t>URL_1_1_1_1_1</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Status_2_1_1_1_1</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Title_1_1_1_1_1_1</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Status_1_1_1_1_1_1</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Title_2_1_1_1_1_1</x:t>
+  </x:si>
+  <x:si>
+    <x:t>URL_1_1_1_1_1_1</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Status_2_1_1_1_1_1</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Title_1_1_1_1_1_1_1</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Status_1_1_1_1_1_1_1</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Title_2_1_1_1_1_1_1</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Status_2_1_1_1_1_1_1</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Trackmania</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.epicgames.com/store/en-US/product/trackmania/home</x:t>
   </x:si>
   <x:si>
     <x:t>Success</x:t>
@@ -412,13 +487,13 @@
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1:L2"/>
+  <x:dimension ref="A1:AK2"/>
   <x:sheetViews>
     <x:sheetView workbookViewId="0"/>
   </x:sheetViews>
   <x:sheetFormatPr defaultRowHeight="15"/>
   <x:sheetData>
-    <x:row r="1" spans="1:12">
+    <x:row r="1" spans="1:37">
       <x:c r="A1" s="0" t="s">
         <x:v>0</x:v>
       </x:c>
@@ -455,22 +530,97 @@
       <x:c r="L1" s="0" t="s">
         <x:v>11</x:v>
       </x:c>
+      <x:c r="M1" s="0" t="s">
+        <x:v>12</x:v>
+      </x:c>
+      <x:c r="N1" s="0" t="s">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="O1" s="0" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="P1" s="0" t="s">
+        <x:v>15</x:v>
+      </x:c>
+      <x:c r="Q1" s="0" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="R1" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="S1" s="0" t="s">
+        <x:v>18</x:v>
+      </x:c>
+      <x:c r="T1" s="0" t="s">
+        <x:v>19</x:v>
+      </x:c>
+      <x:c r="U1" s="0" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="V1" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="W1" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="X1" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="Y1" s="0" t="s">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="Z1" s="0" t="s">
+        <x:v>25</x:v>
+      </x:c>
+      <x:c r="AA1" s="0" t="s">
+        <x:v>26</x:v>
+      </x:c>
+      <x:c r="AB1" s="0" t="s">
+        <x:v>27</x:v>
+      </x:c>
+      <x:c r="AC1" s="0" t="s">
+        <x:v>28</x:v>
+      </x:c>
+      <x:c r="AD1" s="0" t="s">
+        <x:v>29</x:v>
+      </x:c>
+      <x:c r="AE1" s="0" t="s">
+        <x:v>30</x:v>
+      </x:c>
+      <x:c r="AF1" s="0" t="s">
+        <x:v>31</x:v>
+      </x:c>
+      <x:c r="AG1" s="0" t="s">
+        <x:v>32</x:v>
+      </x:c>
+      <x:c r="AH1" s="0" t="s">
+        <x:v>33</x:v>
+      </x:c>
+      <x:c r="AI1" s="0" t="s">
+        <x:v>34</x:v>
+      </x:c>
+      <x:c r="AJ1" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="AK1" s="0" t="s">
+        <x:v>36</x:v>
+      </x:c>
     </x:row>
-    <x:row r="2" spans="1:12">
+    <x:row r="2" spans="1:37">
       <x:c r="A2" s="0" t="s">
-        <x:v>12</x:v>
+        <x:v>37</x:v>
       </x:c>
       <x:c r="B2" s="0" t="s">
-        <x:v>13</x:v>
+        <x:v>38</x:v>
       </x:c>
       <x:c r="C2" s="0" t="s">
-        <x:v>14</x:v>
+        <x:v>39</x:v>
       </x:c>
       <x:c r="D2" s="0" t="s">
-        <x:v>12</x:v>
+        <x:v>37</x:v>
       </x:c>
       <x:c r="E2" s="0" t="s">
-        <x:v>15</x:v>
+        <x:v>40</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>

<commit_message>
Fixed epic adder main
</commit_message>
<xml_diff>
--- a/GameGetter/Data/Input/EpicGameList.xlsx
+++ b/GameGetter/Data/Input/EpicGameList.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
   <x:si>
     <x:t>Title</x:t>
   </x:si>
@@ -124,13 +124,28 @@
     <x:t>Title_2_1_1_1_1_1_1</x:t>
   </x:si>
   <x:si>
+    <x:t>URL_1_1_1_1_1_1_1</x:t>
+  </x:si>
+  <x:si>
     <x:t>Status_2_1_1_1_1_1_1</x:t>
   </x:si>
   <x:si>
-    <x:t>Trackmania</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://www.epicgames.com/store/en-US/product/trackmania/home</x:t>
+    <x:t>Title_1_1_1_1_1_1_1_1</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Status_1_1_1_1_1_1_1_1</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Title_2_1_1_1_1_1_1_1</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Status_2_1_1_1_1_1_1_1</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Might &amp; Magic: Chess Royale</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.epicgames.com/store/en-US/product/might-and-magic-chess-royale</x:t>
   </x:si>
   <x:si>
     <x:t>Success</x:t>
@@ -487,13 +502,13 @@
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1:AK2"/>
+  <x:dimension ref="A1:AP2"/>
   <x:sheetViews>
     <x:sheetView workbookViewId="0"/>
   </x:sheetViews>
   <x:sheetFormatPr defaultRowHeight="15"/>
   <x:sheetData>
-    <x:row r="1" spans="1:37">
+    <x:row r="1" spans="1:42">
       <x:c r="A1" s="0" t="s">
         <x:v>0</x:v>
       </x:c>
@@ -605,22 +620,37 @@
       <x:c r="AK1" s="0" t="s">
         <x:v>36</x:v>
       </x:c>
+      <x:c r="AL1" s="0" t="s">
+        <x:v>37</x:v>
+      </x:c>
+      <x:c r="AM1" s="0" t="s">
+        <x:v>38</x:v>
+      </x:c>
+      <x:c r="AN1" s="0" t="s">
+        <x:v>39</x:v>
+      </x:c>
+      <x:c r="AO1" s="0" t="s">
+        <x:v>40</x:v>
+      </x:c>
+      <x:c r="AP1" s="0" t="s">
+        <x:v>41</x:v>
+      </x:c>
     </x:row>
-    <x:row r="2" spans="1:37">
+    <x:row r="2" spans="1:42">
       <x:c r="A2" s="0" t="s">
-        <x:v>37</x:v>
+        <x:v>42</x:v>
       </x:c>
       <x:c r="B2" s="0" t="s">
-        <x:v>38</x:v>
+        <x:v>43</x:v>
       </x:c>
       <x:c r="C2" s="0" t="s">
-        <x:v>39</x:v>
+        <x:v>44</x:v>
       </x:c>
       <x:c r="D2" s="0" t="s">
-        <x:v>37</x:v>
+        <x:v>42</x:v>
       </x:c>
       <x:c r="E2" s="0" t="s">
-        <x:v>40</x:v>
+        <x:v>45</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>